<commit_message>
second commit : project
</commit_message>
<xml_diff>
--- a/hs_legend.xlsx
+++ b/hs_legend.xlsx
@@ -1284,7 +1284,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>23560</t>
+          <t>25080</t>
         </is>
       </c>
     </row>
@@ -1305,7 +1305,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>11631</t>
+          <t>12422</t>
         </is>
       </c>
     </row>
@@ -1326,7 +1326,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>13028</t>
+          <t>13946</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
3rd commit : project
</commit_message>
<xml_diff>
--- a/hs_legend.xlsx
+++ b/hs_legend.xlsx
@@ -1284,7 +1284,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>25080</t>
+          <t>26649</t>
         </is>
       </c>
     </row>
@@ -1305,7 +1305,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>12422</t>
+          <t>13119</t>
         </is>
       </c>
     </row>
@@ -1326,7 +1326,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>13946</t>
+          <t>14898</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
14th commit : 피드백4 - graph_meta 수정 작업
</commit_message>
<xml_diff>
--- a/hs_legend.xlsx
+++ b/hs_legend.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,6 +448,888 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>108</v>
+      </c>
+      <c r="B2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C2" t="n">
+        <v>10</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>AP</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>7810</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>108</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C3" t="n">
+        <v>10</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>10407</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>108</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C4" t="n">
+        <v>10</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>EU</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>16533</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>109</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C5" t="n">
+        <v>11</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>AP</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>6745</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>109</v>
+      </c>
+      <c r="B6" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C6" t="n">
+        <v>11</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>10260</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>109</v>
+      </c>
+      <c r="B7" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C7" t="n">
+        <v>11</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>EU</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>15820</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>110</v>
+      </c>
+      <c r="B8" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C8" t="n">
+        <v>12</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>AP</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>11005</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>110</v>
+      </c>
+      <c r="B9" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C9" t="n">
+        <v>12</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>18327</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>110</v>
+      </c>
+      <c r="B10" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C10" t="n">
+        <v>12</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>EU</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>23894</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>111</v>
+      </c>
+      <c r="B11" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>AP</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>10129</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>111</v>
+      </c>
+      <c r="B12" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>16942</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>111</v>
+      </c>
+      <c r="B13" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>EU</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>21340</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>112</v>
+      </c>
+      <c r="B14" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C14" t="n">
+        <v>2</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>AP</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>10186</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>112</v>
+      </c>
+      <c r="B15" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>15395</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>112</v>
+      </c>
+      <c r="B16" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C16" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>EU</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>18719</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>113</v>
+      </c>
+      <c r="B17" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C17" t="n">
+        <v>3</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>AP</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>11255</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>113</v>
+      </c>
+      <c r="B18" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C18" t="n">
+        <v>3</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>15265</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>113</v>
+      </c>
+      <c r="B19" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C19" t="n">
+        <v>3</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>EU</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>17902</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>114</v>
+      </c>
+      <c r="B20" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C20" t="n">
+        <v>4</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>AP</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>16265</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>114</v>
+      </c>
+      <c r="B21" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C21" t="n">
+        <v>4</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>20124</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>114</v>
+      </c>
+      <c r="B22" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C22" t="n">
+        <v>4</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>EU</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>23353</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>115</v>
+      </c>
+      <c r="B23" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C23" t="n">
+        <v>5</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>AP</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>16600</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>115</v>
+      </c>
+      <c r="B24" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C24" t="n">
+        <v>5</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>16764</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>115</v>
+      </c>
+      <c r="B25" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C25" t="n">
+        <v>5</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>EU</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>21330</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>116</v>
+      </c>
+      <c r="B26" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C26" t="n">
+        <v>6</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>AP</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>13663</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>116</v>
+      </c>
+      <c r="B27" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C27" t="n">
+        <v>6</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>13130</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>116</v>
+      </c>
+      <c r="B28" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C28" t="n">
+        <v>6</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>EU</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>16598</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>117</v>
+      </c>
+      <c r="B29" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C29" t="n">
+        <v>7</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>AP</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>11625</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>117</v>
+      </c>
+      <c r="B30" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C30" t="n">
+        <v>7</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>10686</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>117</v>
+      </c>
+      <c r="B31" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C31" t="n">
+        <v>7</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>EU</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>12722</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>118</v>
+      </c>
+      <c r="B32" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C32" t="n">
+        <v>8</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>AP</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>21156</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>118</v>
+      </c>
+      <c r="B33" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C33" t="n">
+        <v>8</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>20416</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>118</v>
+      </c>
+      <c r="B34" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C34" t="n">
+        <v>8</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>EU</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>24736</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>119</v>
+      </c>
+      <c r="B35" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C35" t="n">
+        <v>9</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>AP</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>20690</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>119</v>
+      </c>
+      <c r="B36" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C36" t="n">
+        <v>9</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>14868</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>119</v>
+      </c>
+      <c r="B37" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C37" t="n">
+        <v>9</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>EU</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>17818</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>120</v>
+      </c>
+      <c r="B38" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C38" t="n">
+        <v>10</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>AP</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>27168</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>120</v>
+      </c>
+      <c r="B39" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C39" t="n">
+        <v>10</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>15690</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>120</v>
+      </c>
+      <c r="B40" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C40" t="n">
+        <v>10</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>EU</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>17825</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>121</v>
+      </c>
+      <c r="B41" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C41" t="n">
+        <v>11</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>AP</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>41705</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>121</v>
+      </c>
+      <c r="B42" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C42" t="n">
+        <v>11</v>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>20475</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>121</v>
+      </c>
+      <c r="B43" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C43" t="n">
+        <v>11</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>EU</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>22937</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>